<commit_message>
FG configured for output
</commit_message>
<xml_diff>
--- a/example/data/catalogue_list.xlsx
+++ b/example/data/catalogue_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\3.4\PyFDM\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\3.4\PyFDM\example\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="744">
   <si>
     <t>inertial/sea-level-radius_ft</t>
   </si>
@@ -2205,10 +2205,55 @@
     <t>/sim/model/pushback/force</t>
   </si>
   <si>
-    <t>Properties</t>
-  </si>
-  <si>
     <t>RW</t>
+  </si>
+  <si>
+    <t>JSBSIM Properties</t>
+  </si>
+  <si>
+    <t>FG Properties</t>
+  </si>
+  <si>
+    <t>/controls/flight/aileron</t>
+  </si>
+  <si>
+    <t>/controls/flight/elevator</t>
+  </si>
+  <si>
+    <t>/controls/flight/rudder</t>
+  </si>
+  <si>
+    <t>/controls/flight/speedbrake</t>
+  </si>
+  <si>
+    <t>/controls/flight/spoiler</t>
+  </si>
+  <si>
+    <t>/controls/engines/engine/throttle</t>
+  </si>
+  <si>
+    <t>/controls/engines/engine/mixture</t>
+  </si>
+  <si>
+    <t>/controls/flight/flaps</t>
+  </si>
+  <si>
+    <t>/controls/flight/aileron-trim</t>
+  </si>
+  <si>
+    <t>/controls/flight/elevator-trim</t>
+  </si>
+  <si>
+    <t>/controls/flight/rudder-trim</t>
+  </si>
+  <si>
+    <t>/controls/gear/brake-left</t>
+  </si>
+  <si>
+    <t>/controls/gear/brake-right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/controls/gear/steering </t>
   </si>
 </sst>
 </file>
@@ -3017,26 +3062,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:B725"/>
+  <dimension ref="A1:C725"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A182" sqref="A182"/>
+      <selection activeCell="C728" sqref="C728"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B1" t="s">
         <v>727</v>
       </c>
-      <c r="B1" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3044,7 +3093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3052,7 +3101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3060,7 +3109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3068,7 +3117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3076,7 +3125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -3084,7 +3133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -3092,7 +3141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -3100,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -3108,7 +3157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -3116,7 +3165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -3124,7 +3173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -3132,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -3140,7 +3189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -3148,7 +3197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -4308,7 +4357,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>162</v>
       </c>
@@ -4316,7 +4365,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>163</v>
       </c>
@@ -4324,7 +4373,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>164</v>
       </c>
@@ -4332,7 +4381,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>165</v>
       </c>
@@ -4340,7 +4389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>166</v>
       </c>
@@ -4348,7 +4397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>167</v>
       </c>
@@ -4356,79 +4405,106 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B167" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C167" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B168" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C168" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>170</v>
       </c>
       <c r="B169" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C169" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B170" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C170" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>172</v>
       </c>
       <c r="B171" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C171" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>173</v>
       </c>
       <c r="B172" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C172" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>174</v>
       </c>
       <c r="B173" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C173" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B174" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C174" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>176</v>
       </c>
       <c r="B175" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C175" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>177</v>
       </c>
@@ -4564,7 +4640,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>194</v>
       </c>
@@ -4572,7 +4648,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>195</v>
       </c>
@@ -4580,7 +4656,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>196</v>
       </c>
@@ -4588,7 +4664,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>197</v>
       </c>
@@ -4596,7 +4672,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>198</v>
       </c>
@@ -4604,7 +4680,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>199</v>
       </c>
@@ -4612,7 +4688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>200</v>
       </c>
@@ -4620,7 +4696,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>201</v>
       </c>
@@ -4628,7 +4704,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>202</v>
       </c>
@@ -4636,7 +4712,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>203</v>
       </c>
@@ -4644,23 +4720,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>204</v>
       </c>
       <c r="B203" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C203" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>205</v>
       </c>
       <c r="B204" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C204" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>206</v>
       </c>
@@ -4668,15 +4750,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B206" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C206" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>208</v>
       </c>
@@ -4684,15 +4769,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>209</v>
       </c>
       <c r="B208" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C208" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>210</v>
       </c>
@@ -4700,15 +4788,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>211</v>
       </c>
       <c r="B210" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C210" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>212</v>
       </c>
@@ -4716,7 +4807,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>213</v>
       </c>
@@ -4724,7 +4815,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>214</v>
       </c>
@@ -4732,7 +4823,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>215</v>
       </c>
@@ -4740,7 +4831,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>216</v>
       </c>
@@ -4748,7 +4839,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>217</v>
       </c>
@@ -4756,7 +4847,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>218</v>
       </c>
@@ -4764,7 +4855,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>219</v>
       </c>
@@ -4772,7 +4863,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>220</v>
       </c>
@@ -4780,7 +4871,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>221</v>
       </c>
@@ -4788,7 +4879,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>222</v>
       </c>
@@ -4796,7 +4887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>223</v>
       </c>
@@ -4804,7 +4895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>224</v>
       </c>
@@ -4812,7 +4903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>225</v>
       </c>

</xml_diff>